<commit_message>
[expression] - [`nexial.expression.resolveUrl`]: change its default value to `false` to minimize impact to existing automation. This will impact some (likely small subset) of automation that utilize [TEXT expression] to automate the fetching of HTTP-based resources. - [TEXT &raquo; `xml`]: **NEW** operation to transform a [TEXT expression] to a [XML expression]. - [TEXT &raquo; `json`]: **NEW** operation to transform a [TEXT expression] to a [JSON expression].
[external]
- [`runProgram(programPathAndParams)`]: support the execution of sub-shell with parameterized commands (*NIX and Mac only). The parameterized command should be wrapped with single quotes.
- [`runProgramNoWait(programPathAndParams)`]: support the execution of sub-shell with parameterized commands (*NIX and Mac only). The parameterized command should be wrapped with single quotes.

Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/src/test/resources/unittesting/artifact/script/unitTest_buildnum.xlsx
+++ b/src/test/resources/unittesting/artifact/script/unitTest_buildnum.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10908"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ml093043/projects/nexial/nexial-core/src/test/resources/unittesting/artifact/script/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09F5F536-20F8-6641-9D66-77CADB189FB0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89515793-530F-8143-9703-88CC0DE0ABDB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19200" yWindow="-21140" windowWidth="38400" windowHeight="14080" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5120" yWindow="3660" windowWidth="40960" windowHeight="25140" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="#system" sheetId="4" state="hidden" r:id="rId1"/>
@@ -2048,6 +2048,14 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="49" fontId="11" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="49" fontId="7" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
       <protection locked="0"/>
@@ -2075,14 +2083,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -4471,7 +4471,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E16" sqref="E16"/>
+      <selection pane="bottomLeft" activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4492,12 +4492,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="23" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
       <c r="E1" s="24" t="s">
         <v>11</v>
       </c>
@@ -4515,20 +4515,20 @@
       </c>
       <c r="J1" s="19"/>
       <c r="K1" s="3"/>
-      <c r="L1" s="34" t="s">
+      <c r="L1" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="34"/>
-      <c r="N1" s="34"/>
-      <c r="O1" s="35"/>
+      <c r="M1" s="36"/>
+      <c r="N1" s="36"/>
+      <c r="O1" s="37"/>
     </row>
     <row r="2" spans="1:15" ht="93" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="34" t="s">
         <v>549</v>
       </c>
-      <c r="B2" s="33"/>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33"/>
+      <c r="B2" s="35"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
       <c r="E2" s="25"/>
       <c r="F2" s="26"/>
       <c r="G2" s="25"/>
@@ -4538,10 +4538,10 @@
       </c>
       <c r="J2" s="19"/>
       <c r="K2" s="3"/>
-      <c r="L2" s="36"/>
-      <c r="M2" s="37"/>
-      <c r="N2" s="37"/>
-      <c r="O2" s="37"/>
+      <c r="L2" s="38"/>
+      <c r="M2" s="39"/>
+      <c r="N2" s="39"/>
+      <c r="O2" s="39"/>
     </row>
     <row r="3" spans="1:15" ht="10" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="27"/>
@@ -4684,7 +4684,7 @@
     </row>
     <row r="8" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="27"/>
-      <c r="B8" s="38" t="s">
+      <c r="B8" s="30" t="s">
         <v>562</v>
       </c>
       <c r="C8" s="13" t="s">
@@ -4711,7 +4711,7 @@
     </row>
     <row r="9" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="27"/>
-      <c r="B9" s="39"/>
+      <c r="B9" s="31"/>
       <c r="C9" s="13" t="s">
         <v>50</v>
       </c>
@@ -4736,7 +4736,7 @@
     </row>
     <row r="10" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="27"/>
-      <c r="B10" s="39" t="s">
+      <c r="B10" s="31" t="s">
         <v>561</v>
       </c>
       <c r="C10" s="13" t="s">
@@ -4763,7 +4763,7 @@
     </row>
     <row r="11" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="27"/>
-      <c r="B11" s="38" t="s">
+      <c r="B11" s="30" t="s">
         <v>563</v>
       </c>
       <c r="C11" s="13" t="s">
@@ -9776,12 +9776,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="23" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
       <c r="E1" s="29" t="s">
         <v>11</v>
       </c>
@@ -9799,20 +9799,20 @@
       </c>
       <c r="J1" s="19"/>
       <c r="K1" s="3"/>
-      <c r="L1" s="34" t="s">
+      <c r="L1" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="34"/>
-      <c r="N1" s="34"/>
-      <c r="O1" s="35"/>
+      <c r="M1" s="36"/>
+      <c r="N1" s="36"/>
+      <c r="O1" s="37"/>
     </row>
     <row r="2" spans="1:15" ht="93" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="34" t="s">
         <v>549</v>
       </c>
-      <c r="B2" s="33"/>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33"/>
+      <c r="B2" s="35"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
       <c r="E2" s="25"/>
       <c r="F2" s="26"/>
       <c r="G2" s="25"/>
@@ -9822,10 +9822,10 @@
       </c>
       <c r="J2" s="19"/>
       <c r="K2" s="3"/>
-      <c r="L2" s="36"/>
-      <c r="M2" s="37"/>
-      <c r="N2" s="37"/>
-      <c r="O2" s="37"/>
+      <c r="L2" s="38"/>
+      <c r="M2" s="39"/>
+      <c r="N2" s="39"/>
+      <c r="O2" s="39"/>
     </row>
     <row r="3" spans="1:15" ht="10" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="27"/>
@@ -9968,7 +9968,7 @@
     </row>
     <row r="8" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="27"/>
-      <c r="B8" s="38" t="s">
+      <c r="B8" s="30" t="s">
         <v>562</v>
       </c>
       <c r="C8" s="13" t="s">
@@ -9995,7 +9995,7 @@
     </row>
     <row r="9" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="27"/>
-      <c r="B9" s="39"/>
+      <c r="B9" s="31"/>
       <c r="C9" s="13" t="s">
         <v>50</v>
       </c>
@@ -10020,7 +10020,7 @@
     </row>
     <row r="10" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="27"/>
-      <c r="B10" s="39" t="s">
+      <c r="B10" s="31" t="s">
         <v>561</v>
       </c>
       <c r="C10" s="13" t="s">
@@ -10047,7 +10047,7 @@
     </row>
     <row r="11" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="27"/>
-      <c r="B11" s="38" t="s">
+      <c r="B11" s="30" t="s">
         <v>563</v>
       </c>
       <c r="C11" s="13" t="s">

</xml_diff>